<commit_message>
do not disarm and loose key
</commit_message>
<xml_diff>
--- a/doc/modes.xlsx
+++ b/doc/modes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>on*</t>
+  </si>
+  <si>
+    <t>warning, if you disarm by key, SMS is OFF imediatelly, if you disarm by SMS, you have control until sleeep timeout (next five minutes)</t>
   </si>
 </sst>
 </file>
@@ -179,11 +182,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -215,21 +218,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -570,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -581,20 +584,21 @@
     <col min="1" max="1" width="31.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" customWidth="1"/>
+    <col min="8" max="8" width="109.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:8">
+      <c r="C1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -617,8 +621,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -640,8 +644,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:8">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -653,7 +657,7 @@
       <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -662,9 +666,12 @@
       <c r="G4" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:8">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1"/>
@@ -684,8 +691,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="1"/>
@@ -703,8 +710,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:8">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -731,13 +738,13 @@
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="C1:D1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:G7">
+  <conditionalFormatting sqref="C3:G7 H4">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:G7">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="C2:G7 H4">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"n"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>